<commit_message>
va refusals form update
</commit_message>
<xml_diff>
--- a/forms/varefusals/varefusals.xlsx
+++ b/forms/varefusals/varefusals.xlsx
@@ -9,11 +9,11 @@
     <sheet state="visible" name="warnings" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_1DC0C036_1F19_4638_B161_583E5889BA44_.wvu.FilterData">survey!$A$1:$A$26</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_C6F30330_E4DD_4748_B055_8787B1420869_.wvu.FilterData">survey!$A$1:$A$26</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{1DC0C036-1F19-4638-B161-583E5889BA44}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{C6F30330-E4DD-4748-B055-8787B1420869}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -309,7 +309,7 @@
     <t>Can´t find an appropriate respondent</t>
   </si>
   <si>
-    <t>Hawezi kupata mhojiwa mwafaka</t>
+    <t>Mhojiwa sahihi hajapatikana</t>
   </si>
   <si>
     <t>Não consigo encontrar um respondente apropriado</t>
@@ -321,7 +321,7 @@
     <t>Respondent refuses to provide information</t>
   </si>
   <si>
-    <t>Mhojiwa anakataa kutoa habari</t>
+    <t>Mhojiwa amekataa kuhojiwa</t>
   </si>
   <si>
     <t>O entrevistado se recusa a fornecer informações</t>
@@ -333,7 +333,7 @@
     <t>Death doesn’t meet eligibility criteria as per protocol (death &gt;12 months prior visit, deceased was a non-resident, person is alive)</t>
   </si>
   <si>
-    <t>Kifo hakidhi vigezo vya kustahiki kulingana na itifaki (kifo&gt; miezi 12 kabla ya ziara, marehemu hakuwa mkazi, mtu yuko hai</t>
+    <t>Kifo hakijakidhi vigezo stahiki kulingana na itifaki (kifo&gt; miezi 12 kabla ya ziara/marehemu hakuwa mkazi/mtu yuko hai)</t>
   </si>
   <si>
     <t>O óbito não atende aos critérios de elegibilidade de acordo com o protocolo (óbito&gt; 12 meses antes da visita, o falecido era um não residente, pessoa está viva)</t>
@@ -345,7 +345,7 @@
     <t>House destroyed/abandoned</t>
   </si>
   <si>
-    <t>Nyumba kuharibiwa / kutelekezwa</t>
+    <t>Kaya haipo/ Nyumba haina wakazi</t>
   </si>
   <si>
     <t>Casa destruída / abandonada</t>
@@ -973,7 +973,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="17.22"/>
     <col customWidth="1" min="2" max="2" width="24.56"/>
-    <col customWidth="1" min="3" max="3" width="21.22"/>
+    <col customWidth="1" min="3" max="3" width="41.56"/>
     <col customWidth="1" min="4" max="4" width="42.78"/>
     <col customWidth="1" min="5" max="5" width="15.89"/>
     <col customWidth="1" min="6" max="6" width="27.0"/>
@@ -2347,7 +2347,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1DC0C036-1F19-4638-B161-583E5889BA44}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C6F30330-E4DD-4748-B055-8787B1420869}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$A$26"/>
     </customSheetView>
   </customSheetViews>
@@ -2403,7 +2403,8 @@
     <col customWidth="1" min="1" max="1" width="23.56"/>
     <col customWidth="1" min="2" max="2" width="31.89"/>
     <col customWidth="1" min="3" max="3" width="64.56"/>
-    <col customWidth="1" min="4" max="5" width="23.78"/>
+    <col customWidth="1" min="4" max="4" width="88.11"/>
+    <col customWidth="1" min="5" max="5" width="23.78"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2651,7 +2652,7 @@
         <v>126</v>
       </c>
       <c r="F2" s="42">
-        <v>2.021021201E9</v>
+        <v>2.021021902E9</v>
       </c>
     </row>
     <row r="8">

</xml_diff>